<commit_message>
Add SKILL MATRIX AS baseline
Co-Authored-By: ayahamdyahmed <ayahamdyahmed@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Foodies_Documents_Baseline/SKILL-MATRIX.xlsx
+++ b/Foodies_Documents_Baseline/SKILL-MATRIX.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iti\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iti\Documents\GitHub\Foodies\Foodies_Sys_Project_Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A1:AB19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection sqref="A1:O1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,14 +736,14 @@
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="7">
         <v>1</v>
@@ -763,7 +763,7 @@
         <v>1</v>
       </c>
       <c r="P6" s="10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="10">
         <v>1</v>
@@ -777,7 +777,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9">
@@ -840,7 +840,7 @@
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L8" s="7">
         <v>1</v>

</xml_diff>